<commit_message>
Slides for Week 2
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -132,7 +132,8 @@
   <si>
     <t xml:space="preserve">- Scripts vs. Notebooks
 - Take Chances, Make Mistakes, and Get Messy! Don’t be afraid to mess with someone else’s code!
-&lt;div class="tenor-gif-embed" data-postid="5918600078252353803" data-share-method="host" data-aspect-ratio="1.46296" data-width="100%"&gt;&lt;a href="https://tenor.com/view/ms-frizzle-magic-school-bus-gif-5918600078252353803"&gt;Ms Frizzle Magic School Bus GIF&lt;/a&gt;from &lt;a href="https://tenor.com/search/ms+frizzle-gifs"&gt;Ms Frizzle GIFs&lt;/a&gt;&lt;/div&gt; &lt;script type="text/javascript" async src="https://tenor.com/embed.js"&gt;&lt;/script&gt;</t>
+&lt;div class="tenor-gif-embed" data-postid="5918600078252353803" data-share-method="host" data-aspect-ratio="1.46296" data-width="100%"&gt;&lt;a href="https://tenor.com/view/ms-frizzle-magic-school-bus-gif-5918600078252353803"&gt;Ms Frizzle Magic School Bus GIF&lt;/a&gt;from &lt;a href="https://tenor.com/search/ms+frizzle-gifs"&gt;Ms Frizzle GIFs&lt;/a&gt;&lt;/div&gt; &lt;script type="text/javascript" async src="https://tenor.com/embed.js"&gt;&lt;/script&gt;f
+- [Slides](../slides/02-scripts-notebooks.qmd)</t>
   </si>
   <si>
     <r>
@@ -1018,7 +1019,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1055,7 +1056,7 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1082,7 +1083,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="68.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
@@ -1249,7 +1250,7 @@
       <c r="H9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1433,7 +1434,7 @@
       <c r="C17" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I17" s="0" t="s">
+      <c r="I17" s="1" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update slides and docs
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -227,7 +227,7 @@
     <t xml:space="preserve">- [ ] Download and read through the homework assignment</t>
   </si>
   <si>
-    <t xml:space="preserve">- Cues to look for to figure out how code is being run</t>
+    <t xml:space="preserve">- [Cues to look for in Rstudio](../slides/03-intro.qmd)</t>
   </si>
   <si>
     <r>
@@ -1065,7 +1065,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Slides for class today
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -280,7 +280,7 @@
     <t xml:space="preserve">- [ ] Week 4 Reading Quiz</t>
   </si>
   <si>
-    <t xml:space="preserve">- Data Types, Variables, and  Common Mistakes
+    <t xml:space="preserve">- [Data Types, Variables, and  Common Mistakes](../slides/04-building-blocks.qmd)
 - Debugging strategies</t>
   </si>
   <si>
@@ -1064,8 +1064,8 @@
   </sheetPr>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1181,7 +1181,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Course schedule and slide updates
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
   <si>
     <t xml:space="preserve">Week</t>
   </si>
@@ -509,6 +509,10 @@
       <t xml:space="preserve"> half of the semester. 
 - [ ] Homework resubmission deadline is next week! Be sure to finish up any homework you’d like to resubmit. </t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">- [Slides](../slides/07-functions.qmd)
+- [Exam Topics](../slides/08-exam-review.qmd)</t>
   </si>
   <si>
     <r>
@@ -1068,8 +1072,8 @@
   </sheetPr>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1282,8 +1286,11 @@
       <c r="F8" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="G8" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="H8" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1294,17 +1301,17 @@
         <v>45728</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1315,22 +1322,22 @@
         <v>45742</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1341,19 +1348,19 @@
         <v>45749</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1364,22 +1371,22 @@
         <v>45756</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1390,22 +1397,22 @@
         <v>45763</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1416,22 +1423,22 @@
         <v>45770</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1442,22 +1449,22 @@
         <v>45777</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1468,13 +1475,13 @@
         <v>45784</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1485,10 +1492,10 @@
         <v>45791</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for week 11
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -738,7 +738,7 @@
     <t xml:space="preserve">- [ ] Make yourself a cheat sheet of which functions to use for different R and python data manipulation tasks. </t>
   </si>
   <si>
-    <t xml:space="preserve">- Data Cleaning Verbs
+    <t xml:space="preserve">- [Data Cleaning Verbs](../slides/10-wrangling.qmd)
 - Thinking through data processing tasks</t>
   </si>
   <si>
@@ -1077,13 +1077,13 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="34.29"/>
@@ -1368,7 +1368,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Updates for week 14/15
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="93">
   <si>
     <t xml:space="preserve">Week</t>
   </si>
@@ -869,7 +869,7 @@
     <t xml:space="preserve">- [ ] Find an example of a terrible chart in the media</t>
   </si>
   <si>
-    <t xml:space="preserve">- Bad Chart day!</t>
+    <t xml:space="preserve">- [Bad Chart day!](../slides/14-graphics.qmd)</t>
   </si>
   <si>
     <r>
@@ -919,6 +919,46 @@
   </si>
   <si>
     <t xml:space="preserve">- In-class exam review</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- [ ] [Homework 13](../homework/13-practice-final.qmd) </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Submitted via Github classroom</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Finals</t>
@@ -1078,7 +1118,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1489,6 +1529,9 @@
       <c r="G16" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="H16" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -1498,10 +1541,10 @@
         <v>45791</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>